<commit_message>
ENTREGA RF1- añadimos test valores limite, cambio excel y memoria
</commit_message>
<xml_diff>
--- a/docs/EG3_GRUPO_80_11_TestCases.xlsx
+++ b/docs/EG3_GRUPO_80_11_TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzo/Library/Mobile Documents/com~apple~CloudDocs/UC3M/3er Curso/2º Cuatri/Desarrollo de Software/Prácticas/EG3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonsolesmolina/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0005ECEF-C9BE-494F-A7D1-4C554E64EEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A65B6C13-578F-A145-91DB-ADC4C24E3830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cases" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="190">
   <si>
     <t>I/O</t>
   </si>
@@ -136,15 +136,6 @@
     <t>age</t>
   </si>
   <si>
-    <t xml:space="preserve">Carmen Carrero </t>
-  </si>
-  <si>
-    <t>Regular</t>
-  </si>
-  <si>
-    <t>bb5dbd6f-d8b4-413f-8eb9-dd262cfc54e0</t>
-  </si>
-  <si>
     <t>Identificator</t>
   </si>
   <si>
@@ -157,9 +148,6 @@
     <t>CE_NV_03</t>
   </si>
   <si>
-    <t>patient id no es uuid valido (no hex)</t>
-  </si>
-  <si>
     <t>registration_type es otra cosa</t>
   </si>
   <si>
@@ -175,9 +163,6 @@
     <t>patient id es uuid pero version 2</t>
   </si>
   <si>
-    <t>patient id es uuid valido (version 4)</t>
-  </si>
-  <si>
     <t xml:space="preserve">patient id es uuid pero version 1 </t>
   </si>
   <si>
@@ -205,24 +190,15 @@
     <t>CE_NV_12</t>
   </si>
   <si>
-    <t>name_surname con 30 caracteres o menos, en 2 o más cadenas separadas por un blanco</t>
-  </si>
-  <si>
     <t>CE_NV_15</t>
   </si>
   <si>
     <t>CE_NV_16</t>
   </si>
   <si>
-    <t>CE_V_17</t>
-  </si>
-  <si>
     <t>age es int entre 6 y 125</t>
   </si>
   <si>
-    <t>CE_NV_18</t>
-  </si>
-  <si>
     <t>CE_NV_19</t>
   </si>
   <si>
@@ -238,68 +214,826 @@
     <t>SALIDAS</t>
   </si>
   <si>
-    <t>CE_V_21</t>
-  </si>
-  <si>
     <t>MD5 es una cadena hexadecimal</t>
   </si>
   <si>
     <t>MD5 no es una cadena hexadecimal</t>
   </si>
   <si>
-    <t>CE_NV_22</t>
-  </si>
-  <si>
-    <t>CE_V_23</t>
-  </si>
-  <si>
     <t>los datos no son correctos y no se almacenan en el fichero</t>
   </si>
   <si>
-    <t>Family</t>
-  </si>
-  <si>
-    <t>Single</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carmen  </t>
-  </si>
-  <si>
-    <t>Carmen Carrero Rodríguez Fernández Martínez</t>
-  </si>
-  <si>
     <t xml:space="preserve">name_surname con menos de 2 cadenas (sin blanco) </t>
   </si>
   <si>
     <t xml:space="preserve">name_surname con más de 30 caracteres </t>
   </si>
   <si>
-    <t>CE_V_13</t>
-  </si>
-  <si>
-    <t>CE_NV_14</t>
-  </si>
-  <si>
-    <t>teléfono</t>
-  </si>
-  <si>
-    <t>Carmen Carrero</t>
-  </si>
-  <si>
     <t>age es int mayor que 125</t>
   </si>
   <si>
-    <t>diez</t>
-  </si>
-  <si>
     <t>OUTPUT</t>
   </si>
   <si>
     <t>fichero Json</t>
   </si>
   <si>
-    <r>
-      <t>bb5dbd6f-d8b4-</t>
+    <t>registration_type es "Regular"</t>
+  </si>
+  <si>
+    <t>registration_type es "Family"</t>
+  </si>
+  <si>
+    <t>INPUT/OUTPUT</t>
+  </si>
+  <si>
+    <t>CE_NV_25</t>
+  </si>
+  <si>
+    <t>CE_NV_26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone_number no es un número (el string contiene letras) </t>
+  </si>
+  <si>
+    <t>todos los atributos</t>
+  </si>
+  <si>
+    <t>los datos son correctos, no están en el fichero y se almacenan en el fichero</t>
+  </si>
+  <si>
+    <t>test_1</t>
+  </si>
+  <si>
+    <t>test_2</t>
+  </si>
+  <si>
+    <t>test_3</t>
+  </si>
+  <si>
+    <t>test_4</t>
+  </si>
+  <si>
+    <t>test_5</t>
+  </si>
+  <si>
+    <t>test_6</t>
+  </si>
+  <si>
+    <t>test_7</t>
+  </si>
+  <si>
+    <t>test_8</t>
+  </si>
+  <si>
+    <t>test_9</t>
+  </si>
+  <si>
+    <t>test_10</t>
+  </si>
+  <si>
+    <t>test_11</t>
+  </si>
+  <si>
+    <t>test_12</t>
+  </si>
+  <si>
+    <t>test_13</t>
+  </si>
+  <si>
+    <t>test_14</t>
+  </si>
+  <si>
+    <t>test_15</t>
+  </si>
+  <si>
+    <t>test_16</t>
+  </si>
+  <si>
+    <t>test_18</t>
+  </si>
+  <si>
+    <t>los datos son correctos, están en el fichero y no se almacenan en el fichero</t>
+  </si>
+  <si>
+    <t>EC / Valores límite</t>
+  </si>
+  <si>
+    <r>
+      <t>VaccineManagementException (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>"Formato del UUID invalido"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) y el fichero no se crea</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">VaccineManagementException ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>"La edad no es un numero"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) y el fichero no se crea</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">VaccineManagementException ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>"Formato del UUID invalido"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) y el fichero no se crea</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>VaccineManagementException (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>"El Id recibido no es un UUID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) y el fichero no se crea</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>VaccineManagementException (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>"Edad menor de 6 años"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) y el fichero no se crea</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>VaccineManagementException (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>"Tipo de vacunacion solicitada incorrecta"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) y el fichero no se crea</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">VaccineManagementException </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>"Edad mayor de 125 años"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) y el fichero no se crea</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>VaccineManagementException (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>"Cadena sin separacion entre nombre y apellidos"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) y el fichero no se crea</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>VaccineManagementException (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>"Cadena de nombre y apellidos mayor de 30 caracteres"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) y el fichero no se crea</t>
+    </r>
+  </si>
+  <si>
+    <t>age no es un numero (el string contiene letras)</t>
+  </si>
+  <si>
+    <t>los datos no son correctos y se almacenan en el fichero (no se va a dar)</t>
+  </si>
+  <si>
+    <t>Precargamos el fichero con un paciente para probar que el método validate_json_data devuelve False</t>
+  </si>
+  <si>
+    <t>Precargamos el fichero con los mismos datos del paciente para ver que no se vuelve a guardar</t>
+  </si>
+  <si>
+    <r>
+      <t>VaccineManagementException (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>"Formato del UUID invalido"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) y los datos introducidos no se almacenan en el fichero</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>VaccineManagementException (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>"Paciente ya registrado"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) y los datos no se vuelven a almacenar</t>
+    </r>
+  </si>
+  <si>
+    <t>Este test contempla todas las clases de equivalencia válidas, en las que registration_type = “Regular”</t>
+  </si>
+  <si>
+    <t>Este test contempla todas las clases de equivalencia válidas, en las que registration_type = “Family”</t>
+  </si>
+  <si>
+    <t>"+34123456789"</t>
+  </si>
+  <si>
+    <t>"+3412345678"</t>
+  </si>
+  <si>
+    <t>"+341234567899"</t>
+  </si>
+  <si>
+    <t>phone_number es un número de 9 dígitos (a partir de +34)</t>
+  </si>
+  <si>
+    <t>phone_number es un número con menos de 9 dígitos (a partir de +34)</t>
+  </si>
+  <si>
+    <t>phone_number es un número con más de 9 dígitos (a partir de +34)</t>
+  </si>
+  <si>
+    <t>"+34666666666"</t>
+  </si>
+  <si>
+    <t>patient id es uuid valido (de 32 caracteres y version 4)</t>
+  </si>
+  <si>
+    <t>patient id no es uuid valido (no son 32 caracteres o no es hex)</t>
+  </si>
+  <si>
+    <t>EC / Valor límite</t>
+  </si>
+  <si>
+    <t>test_19</t>
+  </si>
+  <si>
+    <t>test_20</t>
+  </si>
+  <si>
+    <t>test_21</t>
+  </si>
+  <si>
+    <t>test_22</t>
+  </si>
+  <si>
+    <t>test_23</t>
+  </si>
+  <si>
+    <t>name_surname de 1 a 30 caracteres, en 2 o más cadenas separadas por un blanco</t>
+  </si>
+  <si>
+    <t>CE_NV_13</t>
+  </si>
+  <si>
+    <t>name_surname con menos de 1 carácter</t>
+  </si>
+  <si>
+    <t>CE_V_14</t>
+  </si>
+  <si>
+    <t>CE_NV_17</t>
+  </si>
+  <si>
+    <t>CE_V_18</t>
+  </si>
+  <si>
+    <t>CE_NV_21</t>
+  </si>
+  <si>
+    <t>CE_V_22</t>
+  </si>
+  <si>
+    <t>CE_NV_23</t>
+  </si>
+  <si>
+    <t>CE_V_24</t>
+  </si>
+  <si>
+    <t>CE_NV_27</t>
+  </si>
+  <si>
+    <t>CE_NV_15. VL = 12 caracteres</t>
+  </si>
+  <si>
+    <t>CE_NV_16. VL = 10 caracteres</t>
+  </si>
+  <si>
+    <t>EC / Valor Límite</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CE_V_18. VL = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">124 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>(por debajo de 125)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CE_NV_06. VL = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">33 caracteres </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>(por encima de 32)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CE_NV_06. VL = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">31 caracteres </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>(por debajo de 32)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CE_NV_12. VL = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">31 caracteres </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>(por encima de 30)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CE_NV_13. VL = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">0 caracteres </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>(por debajo de 1)</t>
+    </r>
+  </si>
+  <si>
+    <t>age, name_surname</t>
+  </si>
+  <si>
+    <t>test_17</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>"Nombre Con Treintayuncaracteres"</t>
+  </si>
+  <si>
+    <t>"C"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Carmen Carrero" </t>
+  </si>
+  <si>
+    <t>"Nombre Veintinueve Caracteres"</t>
+  </si>
+  <si>
+    <t>"Carmen Carrero"</t>
+  </si>
+  <si>
+    <t>"NomTreintacaracteres yunblanco"</t>
+  </si>
+  <si>
+    <t>"C C"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CE_NV_11. VL= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>1 caracter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve"> y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">0 blancos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>(por debajo de 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CE_V_18, CE_V_10. VL =  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">age: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>(por encima de 6),</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> name: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>2 caracteres</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>(por encima de 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CE_NV_20. VL = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>126</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  (por encima de 125)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CE_NV_19. VL = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(por debajo de 6)</t>
+    </r>
+  </si>
+  <si>
+    <t>"Juan Martinez"</t>
+  </si>
+  <si>
+    <t>"22"</t>
+  </si>
+  <si>
+    <t>"7"</t>
+  </si>
+  <si>
+    <t>"5"</t>
+  </si>
+  <si>
+    <t>"124"</t>
+  </si>
+  <si>
+    <t>"126"</t>
+  </si>
+  <si>
+    <t>"diez"</t>
+  </si>
+  <si>
+    <t>"37"</t>
+  </si>
+  <si>
+    <t>"teléfono"</t>
+  </si>
+  <si>
+    <t>"Regular"</t>
+  </si>
+  <si>
+    <t>"Family"</t>
+  </si>
+  <si>
+    <t>"Single"</t>
+  </si>
+  <si>
+    <t>"bb5dbd6f-d8b4-413f-8eb9-dd262cfc54e0"</t>
+  </si>
+  <si>
+    <t>"125"</t>
+  </si>
+  <si>
+    <t>"6"</t>
+  </si>
+  <si>
+    <r>
+      <t>"bb5dbd6f-d8b4-</t>
     </r>
     <r>
       <rPr>
@@ -319,12 +1053,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>13f-8eb9-dd262cfc54e0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>bb5dbd6f-d8b4-</t>
+      <t>13f-8eb9-dd262cfc54e0"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"bb5dbd6f-d8b4-</t>
     </r>
     <r>
       <rPr>
@@ -344,12 +1078,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>13f-8eb9-dd262cfc54e0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>bb5dbd6f-d8b4-</t>
+      <t>13f-8eb9-dd262cfc54e0"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"bb5dbd6f-d8b4-</t>
     </r>
     <r>
       <rPr>
@@ -369,12 +1103,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>13f-8eb9-dd262cfc54e0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>bb5dbd6f-d8b4-</t>
+      <t>13f-8eb9-dd262cfc54e0"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"bb5dbd6f-d8b4-</t>
     </r>
     <r>
       <rPr>
@@ -394,52 +1128,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>13f-8eb9-dd262cfc54e0</t>
-    </r>
-  </si>
-  <si>
-    <t>registration_type es "Regular"</t>
-  </si>
-  <si>
-    <t>registration_type es "Family"</t>
-  </si>
-  <si>
-    <t>CE_V_01, CE_V_07, CE_V_10, CE_V_13, CE_V_17, CE_V_21, CE_V_23</t>
-  </si>
-  <si>
-    <t>CE_V_01, CE_V_08, CE_V_10, CE_V_13, CE_V_17, CE_V_21, CE_V_23</t>
-  </si>
-  <si>
-    <t>CE_NV_24</t>
-  </si>
-  <si>
-    <t>INPUT/OUTPUT</t>
-  </si>
-  <si>
-    <t>CE_NV_25</t>
-  </si>
-  <si>
-    <t>CE_NV_26</t>
-  </si>
-  <si>
-    <t>phone_number es un número de 9 dígitos</t>
-  </si>
-  <si>
-    <t>phone_number es un número con menos de 9 dígitos</t>
-  </si>
-  <si>
-    <t>phone_number es un número con más de 9 dígitos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phone_number no es un número (el string contiene letras) </t>
-  </si>
-  <si>
-    <t>todos los atributos</t>
-  </si>
-  <si>
-    <t>los datos son correctos, no están en el fichero y se almacenan en el fichero</t>
-  </si>
-  <si>
+      <t>13f-8eb9-dd262cfc54e0"</t>
+    </r>
+  </si>
+  <si>
+    <t>"bb5dbd6f-d8b4-413f-8eb9-dd262cfc54e"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>"</t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
@@ -458,75 +1160,68 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>b5dbd6f-d8b4-413f-8eb9-dd262cfc54e0</t>
-    </r>
-  </si>
-  <si>
-    <t>Juan Martínez</t>
-  </si>
-  <si>
-    <t>test_1</t>
-  </si>
-  <si>
-    <t>test_2</t>
-  </si>
-  <si>
-    <t>test_3</t>
-  </si>
-  <si>
-    <t>test_4</t>
-  </si>
-  <si>
-    <t>test_5</t>
-  </si>
-  <si>
-    <t>test_6</t>
-  </si>
-  <si>
-    <t>test_7</t>
-  </si>
-  <si>
-    <t>test_8</t>
-  </si>
-  <si>
-    <t>test_9</t>
-  </si>
-  <si>
-    <t>test_10</t>
-  </si>
-  <si>
-    <t>test_11</t>
-  </si>
-  <si>
-    <t>test_12</t>
-  </si>
-  <si>
-    <t>test_13</t>
-  </si>
-  <si>
-    <t>test_14</t>
-  </si>
-  <si>
-    <t>test_15</t>
-  </si>
-  <si>
-    <t>test_16</t>
-  </si>
-  <si>
-    <t>test_17</t>
-  </si>
-  <si>
-    <t>test_18</t>
-  </si>
-  <si>
-    <t>los datos son correctos, están en el fichero y no se almacenan en el fichero</t>
-  </si>
-  <si>
-    <t>EC / Valores límite</t>
-  </si>
-  <si>
-    <r>
-      <t>cadena hexadecimal válida (</t>
+      <t>b5dbd6f-d8b4-413f-8eb9-dd262cfc54e0"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"bb5dbd6f-d8b4-413f-8eb9-dd262cfc54e0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CE_V_01, CE_V_07, CE_V_10, CE_V_14, CE_V_18, CE_V_22, CE_V_24. VL = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>patient_id: 32 caracteres, name: 30 y 1 blanco, phone: 11, age: 6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CE_V_01, CE_V_08, CE_V_10, CE_V_14, CE_V_18, CE_V_22, CE_V_24. VL = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>name: 29 caracteres (por debajo) y 2 blancos (por encima)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, age: 125</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>VaccineManagementException (</t>
     </r>
     <r>
       <rPr>
@@ -534,7 +1229,7 @@
         <color theme="9" tint="-0.249977111117893"/>
         <rFont val="Calibri (Cuerpo)"/>
       </rPr>
-      <t>b7f631c7c29d52a20b965b5ca7ab6c24</t>
+      <t>"Cadena de nombre vacia"</t>
     </r>
     <r>
       <rPr>
@@ -544,7 +1239,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>) y datos almacenados en fichero</t>
+      <t>) y el fichero no se crea</t>
     </r>
   </si>
   <si>
@@ -557,7 +1252,7 @@
         <color theme="9" tint="-0.249977111117893"/>
         <rFont val="Calibri (Cuerpo)"/>
       </rPr>
-      <t>3467d3fbe384b32f2629074e7db3dd91</t>
+      <t>"0a9d6f313a6355f54caf4cd00a21f2d1"</t>
     </r>
     <r>
       <rPr>
@@ -572,7 +1267,7 @@
   </si>
   <si>
     <r>
-      <t>VaccineManagementException (</t>
+      <t>cadena hexadecimal válida (</t>
     </r>
     <r>
       <rPr>
@@ -580,7 +1275,7 @@
         <color theme="9" tint="-0.249977111117893"/>
         <rFont val="Calibri (Cuerpo)"/>
       </rPr>
-      <t>"Formato del UUID invalido"</t>
+      <t>"44f07ba85efec0a3429b8d732f3c6284"</t>
     </r>
     <r>
       <rPr>
@@ -590,12 +1285,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>) y el fichero no se crea</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">VaccineManagementException ( </t>
+      <t>) y datos almacenados en fichero</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>VaccineManagementException (</t>
     </r>
     <r>
       <rPr>
@@ -603,7 +1298,7 @@
         <color theme="9" tint="-0.249977111117893"/>
         <rFont val="Calibri (Cuerpo)"/>
       </rPr>
-      <t>"La edad no es un numero"</t>
+      <t>"Formato del telefono invalido"</t>
     </r>
     <r>
       <rPr>
@@ -618,7 +1313,24 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">VaccineManagementException ( </t>
+      <t xml:space="preserve">cadena hexadecimal válida </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
     </r>
     <r>
       <rPr>
@@ -626,7 +1338,7 @@
         <color theme="9" tint="-0.249977111117893"/>
         <rFont val="Calibri (Cuerpo)"/>
       </rPr>
-      <t>"Formato del UUID invalido"</t>
+      <t>61fabb7e13e3bb7008e9f247fc982417"</t>
     </r>
     <r>
       <rPr>
@@ -636,12 +1348,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>) y el fichero no se crea</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>VaccineManagementException (</t>
+      <t>) y datos almacenados en fichero</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cadena hexadecimal válida </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
     </r>
     <r>
       <rPr>
@@ -649,7 +1378,7 @@
         <color theme="9" tint="-0.249977111117893"/>
         <rFont val="Calibri (Cuerpo)"/>
       </rPr>
-      <t>"El Id recibido no es un UUID"</t>
+      <t>a1c63840bbf5cf066a2c09d05173595a"</t>
     </r>
     <r>
       <rPr>
@@ -659,278 +1388,36 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>) y el fichero no se crea</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>VaccineManagementException (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>"Edad menor de 6 años"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) y el fichero no se crea</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>VaccineManagementException (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>"Tipo de vacunacion solicitada incorrecta"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) y el fichero no se crea</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">VaccineManagementException </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>"Edad mayor de 125 años"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) y el fichero no se crea</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>VaccineManagementException (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>"Cadena sin separacion entre nombre y apellidos"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) y el fichero no se crea</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>VaccineManagementException (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>"Cadena de nombre y apellidos mayor de 30 caracteres"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) y el fichero no se crea</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>VaccineManagementException (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>"Telefono no es un numero"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) y el fichero no se crea</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>VaccineManagementException (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>"Telefono con menos de 9 digitos"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) y el fichero no se crea</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>VaccineManagementException (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>"Telefono con mas de 9 digitos"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) y el fichero no se crea</t>
-    </r>
-  </si>
-  <si>
-    <t>age no es un numero (el string contiene letras)</t>
-  </si>
-  <si>
-    <t>los datos no son correctos y se almacenan en el fichero (no se va a dar)</t>
-  </si>
-  <si>
-    <t>Precargamos el fichero con un paciente para probar que el método validate_json_data devuelve False</t>
-  </si>
-  <si>
-    <t>Precargamos el fichero con los mismos datos del paciente para ver que no se vuelve a guardar</t>
-  </si>
-  <si>
-    <r>
-      <t>VaccineManagementException (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>"Formato del UUID invalido"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) y los datos introducidos no se almacenan en el fichero</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>VaccineManagementException (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Cuerpo)"/>
-      </rPr>
-      <t>"Paciente ya registrado"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) y los datos no se vuelven a almacenar</t>
-    </r>
-  </si>
-  <si>
-    <t>Este test contempla todas las clases de equivalencia válidas, en las que registration_type = “Regular”</t>
-  </si>
-  <si>
-    <t>Este test contempla todas las clases de equivalencia válidas, en las que registration_type = “Family”</t>
-  </si>
-  <si>
-    <t>Los test 1-2 y 3-16 son parametrizados</t>
+      <t>) y datos almacenados en fichero</t>
+    </r>
+  </si>
+  <si>
+    <t>Los test 1-21 son parametrizados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1037,8 +1524,54 @@
       <color theme="1"/>
       <name val="Calibri (Cuerpo)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1049,6 +1582,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1064,36 +1603,63 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1474,7 +2040,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A1:N42" headerRowDxfId="18" dataDxfId="17" totalsRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A1:N47" headerRowDxfId="18" dataDxfId="17" totalsRowDxfId="16">
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="#" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="I/O" dataDxfId="14"/>
@@ -1726,10 +2292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BDF81A-55AD-44B0-9287-5A7DDAA21E50}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1739,389 +2305,400 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="B5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="15" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="B14" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="B15" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="B16" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B20" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="15" t="s">
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B36" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2132,8 +2709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScale="167" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="J1" zoomScale="75" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2141,14 +2718,14 @@
     <col min="1" max="1" width="10.5703125" style="8" customWidth="1"/>
     <col min="2" max="2" width="13" style="8" customWidth="1"/>
     <col min="3" max="3" width="15" style="8" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="8" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="8" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="49.5703125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="102.5703125" style="8" customWidth="1"/>
     <col min="8" max="8" width="32.42578125" style="8" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" style="8" customWidth="1"/>
     <col min="10" max="10" width="34.140625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="15" style="8" customWidth="1"/>
     <col min="12" max="12" width="5.85546875" style="8" customWidth="1"/>
     <col min="13" max="13" width="85.85546875" style="8" customWidth="1"/>
     <col min="14" max="14" width="77.28515625" style="8" customWidth="1"/>
@@ -2204,88 +2781,88 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" s="24" t="s">
+      <c r="B2" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="8">
-        <v>123456789</v>
-      </c>
-      <c r="L2" s="8">
-        <v>22</v>
-      </c>
-      <c r="M2" s="24" t="s">
-        <v>128</v>
+      <c r="F2" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>184</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="24" t="s">
+      <c r="B3" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="8">
-        <v>123456789</v>
-      </c>
-      <c r="L3" s="8">
-        <v>22</v>
-      </c>
-      <c r="M3" s="24" t="s">
-        <v>127</v>
+      <c r="F3" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="K3" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L3" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="M3" s="28" t="s">
+        <v>185</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2301,35 +2878,35 @@
       <c r="D4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="8">
-        <v>123456789</v>
-      </c>
-      <c r="L4" s="8">
-        <v>22</v>
-      </c>
-      <c r="M4" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="N4" s="25" t="s">
-        <v>149</v>
+      <c r="F4" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="K4" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L4" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2345,32 +2922,32 @@
       <c r="D5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="8">
-        <v>123456789</v>
-      </c>
-      <c r="L5" s="8">
-        <v>22</v>
-      </c>
-      <c r="M5" s="24" t="s">
-        <v>129</v>
+      <c r="F5" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="K5" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L5" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>94</v>
       </c>
       <c r="N5" s="9"/>
     </row>
@@ -2387,32 +2964,32 @@
       <c r="D6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="K6" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="8">
-        <v>123456789</v>
-      </c>
-      <c r="L6" s="8">
-        <v>22</v>
+      <c r="L6" s="39" t="s">
+        <v>160</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2428,32 +3005,32 @@
       <c r="D7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="24" t="s">
-        <v>112</v>
+      <c r="F7" s="21" t="s">
+        <v>80</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="8">
-        <v>123456789</v>
-      </c>
-      <c r="L7" s="8">
-        <v>22</v>
+        <v>40</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="K7" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L7" s="39" t="s">
+        <v>160</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2469,118 +3046,118 @@
       <c r="D8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="24" t="s">
-        <v>113</v>
+      <c r="F8" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="8">
-        <v>123456789</v>
-      </c>
-      <c r="L8" s="8">
-        <v>22</v>
+        <v>38</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="K8" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L8" s="39" t="s">
+        <v>160</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="N8" s="9"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
+      <c r="A9" s="29">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="8" t="s">
+      <c r="C9" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="9">
-        <v>123456789</v>
-      </c>
-      <c r="L9" s="8">
-        <v>22</v>
+      <c r="F9" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="J9" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="K9" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L9" s="39" t="s">
+        <v>160</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N9" s="9"/>
+        <v>97</v>
+      </c>
+      <c r="N9" s="25"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
+      <c r="A10" s="29">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="8" t="s">
+      <c r="C10" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="K10" s="9">
-        <v>123456789</v>
-      </c>
-      <c r="L10" s="8">
-        <v>22</v>
+      <c r="F10" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="K10" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L10" s="39" t="s">
+        <v>160</v>
       </c>
       <c r="M10" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="N10" s="9"/>
+        <v>97</v>
+      </c>
+      <c r="N10" s="25"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
@@ -2593,34 +3170,34 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="K11" s="9">
-        <v>123456789</v>
-      </c>
-      <c r="L11" s="8">
-        <v>22</v>
-      </c>
-      <c r="M11" s="24" t="s">
-        <v>137</v>
+        <v>84</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J11" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="K11" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L11" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="M11" s="21" t="s">
+        <v>99</v>
       </c>
       <c r="N11" s="9"/>
     </row>
@@ -2631,124 +3208,124 @@
       <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>126</v>
+      <c r="C12" s="28" t="s">
+        <v>120</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K12" s="11">
-        <v>12345678</v>
-      </c>
-      <c r="L12" s="8">
-        <v>22</v>
-      </c>
-      <c r="M12" s="24" t="s">
-        <v>139</v>
+        <v>85</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L12" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>101</v>
       </c>
       <c r="N12" s="9"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
+      <c r="A13" s="29">
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>126</v>
+      <c r="C13" s="28" t="s">
+        <v>120</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13" s="11">
-        <v>1234567899</v>
-      </c>
-      <c r="L13" s="8">
-        <v>22</v>
-      </c>
-      <c r="M13" s="24" t="s">
-        <v>140</v>
+      <c r="F13" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K13" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L13" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="M13" s="21" t="s">
+        <v>102</v>
       </c>
       <c r="N13" s="9"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
+      <c r="A14" s="24">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>8</v>
+      <c r="C14" s="28" t="s">
+        <v>120</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="L14" s="8">
-        <v>22</v>
-      </c>
-      <c r="M14" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="N14" s="9"/>
+      <c r="F14" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="K14" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L14" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="M14" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="N14" s="25"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
@@ -2757,38 +3334,38 @@
       <c r="B15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>126</v>
+      <c r="C15" s="24" t="s">
+        <v>120</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>61</v>
+        <v>88</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>137</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>34</v>
+        <v>171</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>168</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="K15" s="9">
-        <v>123456789</v>
-      </c>
-      <c r="L15" s="11">
-        <v>5</v>
-      </c>
-      <c r="M15" s="24" t="s">
-        <v>133</v>
+        <v>150</v>
+      </c>
+      <c r="K15" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="L15" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="M15" s="28" t="s">
+        <v>186</v>
       </c>
       <c r="N15" s="9"/>
     </row>
@@ -2799,38 +3376,38 @@
       <c r="B16" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>126</v>
+      <c r="C16" s="24" t="s">
+        <v>120</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>62</v>
+        <v>89</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>138</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="K16" s="9">
-        <v>123456789</v>
-      </c>
-      <c r="L16" s="11">
-        <v>126</v>
-      </c>
-      <c r="M16" s="24" t="s">
-        <v>135</v>
+        <v>171</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="K16" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="L16" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="M16" s="28" t="s">
+        <v>186</v>
       </c>
       <c r="N16" s="9"/>
     </row>
@@ -2845,221 +3422,355 @@
         <v>8</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>64</v>
+        <v>90</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>130</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>34</v>
+        <v>171</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>168</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="K17" s="9">
-        <v>123456789</v>
-      </c>
-      <c r="L17" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="M17" s="24" t="s">
-        <v>130</v>
+        <v>152</v>
+      </c>
+      <c r="K17" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="L17" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="M17" s="28" t="s">
+        <v>186</v>
       </c>
       <c r="N17" s="9"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="8">
+      <c r="A18" s="24">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>87</v>
+      <c r="B18" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>171</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="K18" s="9">
-        <v>666666666</v>
-      </c>
-      <c r="L18" s="9">
-        <v>37</v>
-      </c>
-      <c r="M18" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="N18" s="9" t="s">
-        <v>143</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="J18" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="K18" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L18" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="M18" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="N18" s="25"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I19" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K19" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L19" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="N19" s="9"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="24">
+        <v>19</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="K20" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L20" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="M20" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="N20" s="25"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K21" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L21" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="M21" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="N21" s="9"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="24" t="s">
+      <c r="D22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F22" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="J22" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="K22" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L22" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="M22" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="N22" s="9"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="G19" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="I19" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="J19" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="K19" s="24">
-        <v>123456789</v>
-      </c>
-      <c r="L19" s="9">
-        <v>22</v>
-      </c>
-      <c r="M19" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="N19" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="9"/>
-    </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-    </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-    </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
+      <c r="G23" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="I23" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="K23" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="L23" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="M23" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
+      <c r="A24" s="8">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="I24" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="J24" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="K24" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L24" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="M24" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="N24" s="9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
+      <c r="K25" s="21"/>
       <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
+      <c r="M25" s="21"/>
       <c r="N25" s="9"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
@@ -3073,9 +3784,7 @@
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
@@ -3091,7 +3800,6 @@
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
@@ -3107,7 +3815,6 @@
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
@@ -3321,11 +4028,86 @@
       <c r="M42" s="9"/>
       <c r="N42" s="9"/>
     </row>
-    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+    </row>
+    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9"/>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+    </row>
     <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>